<commit_message>
NSE-7719 - completed the addition of the admins for every repo
</commit_message>
<xml_diff>
--- a/NEONScience/NEONScience_Repos.xlsx
+++ b/NEONScience/NEONScience_Repos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Common\CI\NEONScience\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhayes\JIRA-Tickets\NSE-7719\NEONIT\NEONScience\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FAD331-6AA3-40DC-A2D7-33CB8398D246}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3F0C8E-CFAF-4607-9EBF-377572479EFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="4845" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4020" yWindow="3210" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="newrepos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="446">
   <si>
     <t>Repo Name</t>
   </si>
@@ -1182,12 +1182,6 @@
   <si>
     <t>Allan Schmidt
 Eve Lempriere</t>
-  </si>
-  <si>
-    <t>Samantha Weintraub</t>
-  </si>
-  <si>
-    <t>Committers</t>
   </si>
   <si>
     <t>David Durden
@@ -1235,6 +1229,260 @@
     <t>Claire Lunch
 Caren Scott
 Eric Sokol</t>
+  </si>
+  <si>
+    <t>Cody Flagg
+Katie Jones
+Natalie Robinson</t>
+  </si>
+  <si>
+    <t>Claire Lunch
+Christine Laney
+Allan Schmidt</t>
+  </si>
+  <si>
+    <t>Josh Roberti
+Robert Lee</t>
+  </si>
+  <si>
+    <t>Stefan Metzger
+David Durden</t>
+  </si>
+  <si>
+    <t>Cody Flagg
+Caren Scott
+Jim Coloso</t>
+  </si>
+  <si>
+    <t>Cody Flagg
+mariefs93</t>
+  </si>
+  <si>
+    <t>mariefs93 is an outside collaborator</t>
+  </si>
+  <si>
+    <t>Katie LeVan
+Cody Flagg</t>
+  </si>
+  <si>
+    <t>Hongyan Luo
+Robert Lee</t>
+  </si>
+  <si>
+    <t>Claire Lunch
+Bobby Hensley
+Ross Gaddie
+Kaelin Cawley</t>
+  </si>
+  <si>
+    <t>Kate Thibault
+Katie LeVan</t>
+  </si>
+  <si>
+    <t>Kate LeVan</t>
+  </si>
+  <si>
+    <t>Claire Lunch
+Cove Sturtevant</t>
+  </si>
+  <si>
+    <t>Katie Jones</t>
+  </si>
+  <si>
+    <t>Katie Jones
+Eve Lempriere
+Allan Schmidt</t>
+  </si>
+  <si>
+    <t>Guy Litt</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>This was setup by Greg Holling and there is nothing in the repo</t>
+  </si>
+  <si>
+    <t>Eric Sokol</t>
+  </si>
+  <si>
+    <t>Stefan Metzer
+David Durden
+Ke Xu
+Cove Sturtevant
+Hongyan Luo
+Robert Lee
+Chris Florian</t>
+  </si>
+  <si>
+    <t>33 admins</t>
+  </si>
+  <si>
+    <t>Cody Flagg
+jcoloso
+mariefst93</t>
+  </si>
+  <si>
+    <t>jcoloso and mariefst93 are outside collaborators</t>
+  </si>
+  <si>
+    <t>Cove Sturtevant
+Kaelin Cawley
+Dawn Lenz
+Rob Markel</t>
+  </si>
+  <si>
+    <t>This can probably be deleted. I'll ask Cove</t>
+  </si>
+  <si>
+    <t>Teresa Burlingame
+Caren Scott
+Kaelin Cawley
+Christine Laney</t>
+  </si>
+  <si>
+    <t>Caren Scott
+Christine Laney
+Claire Lunch</t>
+  </si>
+  <si>
+    <t>Christine Laney
+Claire Lunch
+Dawn Lenz</t>
+  </si>
+  <si>
+    <t>Katie LeVan
+Eric Sokol</t>
+  </si>
+  <si>
+    <t>Claire Lunch
+Eric Sokol
+Caren Scott</t>
+  </si>
+  <si>
+    <t>Kate Thibault
+Courtney Meier
+Eric Sokol
+Stephanie Parker</t>
+  </si>
+  <si>
+    <t>Edward Ayres
+Josh Roberti
+Claire Lunch
+Christine Laney</t>
+  </si>
+  <si>
+    <t>Caren Scott</t>
+  </si>
+  <si>
+    <t>Cody Flagg
+Natalie Robinson
+Katie LeVan
+Josh Roberti
+Robert Lee
+Kevin Styers</t>
+  </si>
+  <si>
+    <t>Caren Scott
+Claire Lunch
+Eric Sokol</t>
+  </si>
+  <si>
+    <t>Cody Flagg
+Katie LeVan</t>
+  </si>
+  <si>
+    <t>Caren Scott
+Cody Flagg
+Geoffrey House
+Samantha Weintraub</t>
+  </si>
+  <si>
+    <t>Cody Flagg
+Jeremy Sampson</t>
+  </si>
+  <si>
+    <t>Christopher Clark
+Jeremy Sampson
+Cody Flagg</t>
+  </si>
+  <si>
+    <t>Kevin Styers
+robhamnett</t>
+  </si>
+  <si>
+    <t>robhamnet is an outside collaborator.</t>
+  </si>
+  <si>
+    <t>Geoffrey House</t>
+  </si>
+  <si>
+    <t>Dawn Lenz
+Chris Florian
+Claire Lunch
+Christine Laney
+Cove Sturtevant</t>
+  </si>
+  <si>
+    <t>Christine Laney
+Stefan Metzer</t>
+  </si>
+  <si>
+    <t>Natalie Robinson
+Eric Sokol</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>empty created by Lee Stanish</t>
+  </si>
+  <si>
+    <t>Stefan Metzer
+Cove Sturtevant
+Katie LeVan
+Cody Flagg</t>
+  </si>
+  <si>
+    <t>Cody Flagg
+Sara Paull
+jcoloso
+tgilbert14</t>
+  </si>
+  <si>
+    <t>jcoloso and tgilbert14 are outside collaborators</t>
+  </si>
+  <si>
+    <t>Cody Flagg
+Christine Laney
+Kaelin Cawley
+Katie LeVan</t>
+  </si>
+  <si>
+    <t>Kate Thibault
+Courtney Meier</t>
+  </si>
+  <si>
+    <t>Eve Lempriere
+Allan Schmidt</t>
+  </si>
+  <si>
+    <t>This was Lee Standish's repo. It needs an owner</t>
+  </si>
+  <si>
+    <t>Cody Flagg
+Kevin Styers
+Natalie Robinson
+rkieferbattelle</t>
+  </si>
+  <si>
+    <t>rkieferbattelle is Ryan Kiefer in IT and is an outside collaborator for this repo.</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Samantha Weintraub is the main committer</t>
   </si>
 </sst>
 </file>
@@ -1718,11 +1966,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2082,8 +2333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,7 +2345,7 @@
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2117,8 +2368,8 @@
       <c r="F1" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>380</v>
+      <c r="G1" s="4" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2180,7 +2431,6 @@
       <c r="F4" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3143,7 +3393,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>17</v>
       </c>
@@ -3162,8 +3412,8 @@
       <c r="F53" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="G53" t="s">
-        <v>379</v>
+      <c r="G53" s="3" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -3183,7 +3433,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3223,7 +3473,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3243,7 +3493,7 @@
         <v>1</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3323,7 +3573,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3383,7 +3633,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3403,7 +3653,7 @@
         <v>1</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3423,7 +3673,7 @@
         <v>1</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3443,7 +3693,7 @@
         <v>1</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3483,10 +3733,10 @@
         <v>1</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>39</v>
       </c>
@@ -3502,9 +3752,11 @@
       <c r="E70" t="b">
         <v>1</v>
       </c>
-      <c r="F70" s="3"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F70" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>45</v>
       </c>
@@ -3520,9 +3772,11 @@
       <c r="E71" t="b">
         <v>1</v>
       </c>
-      <c r="F71" s="3"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F71" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>7</v>
       </c>
@@ -3538,9 +3792,11 @@
       <c r="E72" t="b">
         <v>1</v>
       </c>
-      <c r="F72" s="3"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F72" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>247</v>
       </c>
@@ -3556,7 +3812,9 @@
       <c r="E73" t="b">
         <v>1</v>
       </c>
-      <c r="F73" s="3"/>
+      <c r="F73" s="3" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
@@ -3574,7 +3832,9 @@
       <c r="E74" t="b">
         <v>1</v>
       </c>
-      <c r="F74" s="3"/>
+      <c r="F74" s="3" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
@@ -3592,7 +3852,9 @@
       <c r="E75" t="b">
         <v>1</v>
       </c>
-      <c r="F75" s="3"/>
+      <c r="F75" s="3" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
@@ -3610,7 +3872,9 @@
       <c r="E76" t="b">
         <v>1</v>
       </c>
-      <c r="F76" s="3"/>
+      <c r="F76" s="3" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
@@ -3628,7 +3892,9 @@
       <c r="E77" t="b">
         <v>1</v>
       </c>
-      <c r="F77" s="3"/>
+      <c r="F77" s="3" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
@@ -3646,9 +3912,11 @@
       <c r="E78" t="b">
         <v>1</v>
       </c>
-      <c r="F78" s="3"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F78" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>41</v>
       </c>
@@ -3664,9 +3932,11 @@
       <c r="E79" t="b">
         <v>1</v>
       </c>
-      <c r="F79" s="3"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F79" s="3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>273</v>
       </c>
@@ -3682,9 +3952,11 @@
       <c r="E80" t="b">
         <v>1</v>
       </c>
-      <c r="F80" s="3"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F80" s="3" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>113</v>
       </c>
@@ -3700,9 +3972,11 @@
       <c r="E81" t="b">
         <v>1</v>
       </c>
-      <c r="F81" s="3"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F81" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>261</v>
       </c>
@@ -3718,9 +3992,11 @@
       <c r="E82" t="b">
         <v>1</v>
       </c>
-      <c r="F82" s="3"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F82" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>107</v>
       </c>
@@ -3736,9 +4012,11 @@
       <c r="E83" t="b">
         <v>1</v>
       </c>
-      <c r="F83" s="3"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F83" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>339</v>
       </c>
@@ -3754,9 +4032,11 @@
       <c r="E84" t="b">
         <v>1</v>
       </c>
-      <c r="F84" s="3"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>329</v>
       </c>
@@ -3772,9 +4052,11 @@
       <c r="E85" t="b">
         <v>1</v>
       </c>
-      <c r="F85" s="3"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F85" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>297</v>
       </c>
@@ -3790,9 +4072,11 @@
       <c r="E86" t="b">
         <v>1</v>
       </c>
-      <c r="F86" s="3"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>275</v>
       </c>
@@ -3808,9 +4092,14 @@
       <c r="E87" t="b">
         <v>1</v>
       </c>
-      <c r="F87" s="3"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F87" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>211</v>
       </c>
@@ -3826,9 +4115,11 @@
       <c r="E88" t="b">
         <v>1</v>
       </c>
-      <c r="F88" s="3"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F88" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>263</v>
       </c>
@@ -3844,9 +4135,11 @@
       <c r="E89" t="b">
         <v>1</v>
       </c>
-      <c r="F89" s="3"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F89" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>53</v>
       </c>
@@ -3862,9 +4155,11 @@
       <c r="E90" t="b">
         <v>1</v>
       </c>
-      <c r="F90" s="3"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F90" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>163</v>
       </c>
@@ -3880,9 +4175,11 @@
       <c r="E91" t="b">
         <v>1</v>
       </c>
-      <c r="F91" s="3"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F91" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>19</v>
       </c>
@@ -3898,9 +4195,11 @@
       <c r="E92" t="b">
         <v>1</v>
       </c>
-      <c r="F92" s="3"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F92" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>317</v>
       </c>
@@ -3916,9 +4215,11 @@
       <c r="E93" t="b">
         <v>1</v>
       </c>
-      <c r="F93" s="3"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F93" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>191</v>
       </c>
@@ -3934,9 +4235,11 @@
       <c r="E94" t="b">
         <v>1</v>
       </c>
-      <c r="F94" s="3"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F94" s="3" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>49</v>
       </c>
@@ -3952,9 +4255,11 @@
       <c r="E95" t="b">
         <v>1</v>
       </c>
-      <c r="F95" s="3"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F95" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>141</v>
       </c>
@@ -3970,9 +4275,11 @@
       <c r="E96" t="b">
         <v>1</v>
       </c>
-      <c r="F96" s="3"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F96" s="3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>21</v>
       </c>
@@ -3988,9 +4295,11 @@
       <c r="E97" t="b">
         <v>1</v>
       </c>
-      <c r="F97" s="3"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F97" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>195</v>
       </c>
@@ -4006,9 +4315,11 @@
       <c r="E98" t="b">
         <v>1</v>
       </c>
-      <c r="F98" s="3"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F98" s="3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>291</v>
       </c>
@@ -4024,9 +4335,11 @@
       <c r="E99" t="b">
         <v>1</v>
       </c>
-      <c r="F99" s="3"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F99" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>207</v>
       </c>
@@ -4042,9 +4355,11 @@
       <c r="E100" t="b">
         <v>1</v>
       </c>
-      <c r="F100" s="3"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F100" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>125</v>
       </c>
@@ -4060,9 +4375,11 @@
       <c r="E101" t="b">
         <v>1</v>
       </c>
-      <c r="F101" s="3"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F101" s="3" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>129</v>
       </c>
@@ -4078,9 +4395,11 @@
       <c r="E102" t="b">
         <v>1</v>
       </c>
-      <c r="F102" s="3"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F102" s="3" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>33</v>
       </c>
@@ -4096,9 +4415,14 @@
       <c r="E103" t="b">
         <v>1</v>
       </c>
-      <c r="F103" s="3"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F103" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>315</v>
       </c>
@@ -4114,9 +4438,11 @@
       <c r="E104" t="b">
         <v>1</v>
       </c>
-      <c r="F104" s="3"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F104" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>239</v>
       </c>
@@ -4132,9 +4458,11 @@
       <c r="E105" t="b">
         <v>1</v>
       </c>
-      <c r="F105" s="3"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F105" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>13</v>
       </c>
@@ -4150,9 +4478,11 @@
       <c r="E106" t="b">
         <v>1</v>
       </c>
-      <c r="F106" s="3"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F106" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>155</v>
       </c>
@@ -4168,9 +4498,11 @@
       <c r="E107" t="b">
         <v>1</v>
       </c>
-      <c r="F107" s="3"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F107" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>165</v>
       </c>
@@ -4186,9 +4518,11 @@
       <c r="E108" t="b">
         <v>1</v>
       </c>
-      <c r="F108" s="3"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F108" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>73</v>
       </c>
@@ -4204,9 +4538,14 @@
       <c r="E109" t="b">
         <v>1</v>
       </c>
-      <c r="F109" s="3"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F109" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>35</v>
       </c>
@@ -4222,9 +4561,11 @@
       <c r="E110" t="b">
         <v>1</v>
       </c>
-      <c r="F110" s="3"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F110" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>5</v>
       </c>
@@ -4240,9 +4581,11 @@
       <c r="E111" t="b">
         <v>1</v>
       </c>
-      <c r="F111" s="3"/>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F111" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>43</v>
       </c>
@@ -4258,9 +4601,11 @@
       <c r="E112" t="b">
         <v>1</v>
       </c>
-      <c r="F112" s="3"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F112" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>287</v>
       </c>
@@ -4276,9 +4621,11 @@
       <c r="E113" t="b">
         <v>1</v>
       </c>
-      <c r="F113" s="3"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F113" s="3" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>31</v>
       </c>
@@ -4294,9 +4641,11 @@
       <c r="E114" t="b">
         <v>1</v>
       </c>
-      <c r="F114" s="3"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F114" s="3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>23</v>
       </c>
@@ -4312,9 +4661,14 @@
       <c r="E115" t="b">
         <v>1</v>
       </c>
-      <c r="F115" s="3"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F115" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>171</v>
       </c>
@@ -4330,9 +4684,11 @@
       <c r="E116" t="b">
         <v>1</v>
       </c>
-      <c r="F116" s="3"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F116" s="3" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>271</v>
       </c>
@@ -4348,9 +4704,14 @@
       <c r="E117" t="b">
         <v>1</v>
       </c>
-      <c r="F117" s="3"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F117" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>57</v>
       </c>
@@ -4366,9 +4727,11 @@
       <c r="E118" t="b">
         <v>1</v>
       </c>
-      <c r="F118" s="3"/>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F118" s="3" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>205</v>
       </c>
@@ -4384,9 +4747,11 @@
       <c r="E119" t="b">
         <v>1</v>
       </c>
-      <c r="F119" s="3"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F119" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>189</v>
       </c>
@@ -4402,9 +4767,14 @@
       <c r="E120" t="b">
         <v>1</v>
       </c>
-      <c r="F120" s="3"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F120" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>313</v>
       </c>
@@ -4420,9 +4790,11 @@
       <c r="E121" t="b">
         <v>1</v>
       </c>
-      <c r="F121" s="3"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F121" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -4438,9 +4810,11 @@
       <c r="E122" t="b">
         <v>1</v>
       </c>
-      <c r="F122" s="3"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F122" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>61</v>
       </c>
@@ -4456,9 +4830,11 @@
       <c r="E123" t="b">
         <v>1</v>
       </c>
-      <c r="F123" s="3"/>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F123" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>137</v>
       </c>
@@ -4474,9 +4850,11 @@
       <c r="E124" t="b">
         <v>1</v>
       </c>
-      <c r="F124" s="3"/>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F124" s="3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>255</v>
       </c>
@@ -4492,9 +4870,11 @@
       <c r="E125" t="b">
         <v>1</v>
       </c>
-      <c r="F125" s="3"/>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F125" s="3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>151</v>
       </c>
@@ -4510,9 +4890,11 @@
       <c r="E126" t="b">
         <v>1</v>
       </c>
-      <c r="F126" s="3"/>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F126" s="3" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>217</v>
       </c>
@@ -4528,9 +4910,11 @@
       <c r="E127" t="b">
         <v>1</v>
       </c>
-      <c r="F127" s="3"/>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F127" s="3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>147</v>
       </c>
@@ -4546,9 +4930,11 @@
       <c r="E128" t="b">
         <v>1</v>
       </c>
-      <c r="F128" s="3"/>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F128" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>97</v>
       </c>
@@ -4564,9 +4950,11 @@
       <c r="E129" t="b">
         <v>1</v>
       </c>
-      <c r="F129" s="3"/>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F129" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>27</v>
       </c>
@@ -4582,9 +4970,11 @@
       <c r="E130" t="b">
         <v>1</v>
       </c>
-      <c r="F130" s="3"/>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F130" s="3" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>119</v>
       </c>
@@ -4600,9 +4990,11 @@
       <c r="E131" t="b">
         <v>1</v>
       </c>
-      <c r="F131" s="3"/>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F131" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>181</v>
       </c>
@@ -4618,9 +5010,11 @@
       <c r="E132" t="b">
         <v>1</v>
       </c>
-      <c r="F132" s="3"/>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F132" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>77</v>
       </c>
@@ -4636,9 +5030,11 @@
       <c r="E133" t="b">
         <v>1</v>
       </c>
-      <c r="F133" s="3"/>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F133" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>219</v>
       </c>
@@ -4654,9 +5050,11 @@
       <c r="E134" t="b">
         <v>1</v>
       </c>
-      <c r="F134" s="3"/>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F134" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>9</v>
       </c>
@@ -4672,9 +5070,11 @@
       <c r="E135" t="b">
         <v>1</v>
       </c>
-      <c r="F135" s="3"/>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F135" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>161</v>
       </c>
@@ -4690,9 +5090,11 @@
       <c r="E136" t="b">
         <v>1</v>
       </c>
-      <c r="F136" s="3"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F136" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>259</v>
       </c>
@@ -4708,9 +5110,11 @@
       <c r="E137" t="b">
         <v>1</v>
       </c>
-      <c r="F137" s="3"/>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F137" s="3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>187</v>
       </c>
@@ -4726,9 +5130,11 @@
       <c r="E138" t="b">
         <v>1</v>
       </c>
-      <c r="F138" s="3"/>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F138" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>131</v>
       </c>
@@ -4744,9 +5150,11 @@
       <c r="E139" t="b">
         <v>1</v>
       </c>
-      <c r="F139" s="3"/>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F139" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>235</v>
       </c>
@@ -4762,9 +5170,11 @@
       <c r="E140" t="b">
         <v>1</v>
       </c>
-      <c r="F140" s="3"/>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F140" s="3" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>231</v>
       </c>
@@ -4780,9 +5190,11 @@
       <c r="E141" t="b">
         <v>1</v>
       </c>
-      <c r="F141" s="3"/>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F141" s="3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>277</v>
       </c>
@@ -4798,9 +5210,11 @@
       <c r="E142" t="b">
         <v>1</v>
       </c>
-      <c r="F142" s="3"/>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F142" s="3" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>281</v>
       </c>
@@ -4816,9 +5230,14 @@
       <c r="E143" t="b">
         <v>1</v>
       </c>
-      <c r="F143" s="3"/>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F143" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="G143" s="3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>307</v>
       </c>
@@ -4834,9 +5253,11 @@
       <c r="E144" t="b">
         <v>1</v>
       </c>
-      <c r="F144" s="3"/>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F144" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>335</v>
       </c>
@@ -4852,9 +5273,11 @@
       <c r="E145" t="b">
         <v>1</v>
       </c>
-      <c r="F145" s="3"/>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F145" s="3" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>55</v>
       </c>
@@ -4870,9 +5293,11 @@
       <c r="E146" t="b">
         <v>1</v>
       </c>
-      <c r="F146" s="3"/>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F146" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>169</v>
       </c>
@@ -4888,9 +5313,11 @@
       <c r="E147" t="b">
         <v>1</v>
       </c>
-      <c r="F147" s="3"/>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F147" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>267</v>
       </c>
@@ -4906,9 +5333,11 @@
       <c r="E148" t="b">
         <v>1</v>
       </c>
-      <c r="F148" s="3"/>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F148" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>257</v>
       </c>
@@ -4924,9 +5353,11 @@
       <c r="E149" t="b">
         <v>1</v>
       </c>
-      <c r="F149" s="3"/>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F149" s="3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>83</v>
       </c>
@@ -4942,9 +5373,14 @@
       <c r="E150" t="b">
         <v>1</v>
       </c>
-      <c r="F150" s="3"/>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F150" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>341</v>
       </c>
@@ -4960,9 +5396,11 @@
       <c r="E151" t="b">
         <v>1</v>
       </c>
-      <c r="F151" s="3"/>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F151" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>103</v>
       </c>
@@ -4978,9 +5416,11 @@
       <c r="E152" t="b">
         <v>1</v>
       </c>
-      <c r="F152" s="3"/>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F152" s="3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>123</v>
       </c>
@@ -4996,9 +5436,11 @@
       <c r="E153" t="b">
         <v>1</v>
       </c>
-      <c r="F153" s="3"/>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F153" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>305</v>
       </c>
@@ -5014,9 +5456,14 @@
       <c r="E154" t="b">
         <v>1</v>
       </c>
-      <c r="F154" s="3"/>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F154" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>243</v>
       </c>
@@ -5032,9 +5479,11 @@
       <c r="E155" t="b">
         <v>1</v>
       </c>
-      <c r="F155" s="3"/>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F155" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>115</v>
       </c>
@@ -5050,9 +5499,11 @@
       <c r="E156" t="b">
         <v>1</v>
       </c>
-      <c r="F156" s="3"/>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F156" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>93</v>
       </c>
@@ -5068,9 +5519,11 @@
       <c r="E157" t="b">
         <v>1</v>
       </c>
-      <c r="F157" s="3"/>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F157" s="3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>127</v>
       </c>
@@ -5086,9 +5539,11 @@
       <c r="E158" t="b">
         <v>1</v>
       </c>
-      <c r="F158" s="3"/>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F158" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>81</v>
       </c>
@@ -5104,9 +5559,11 @@
       <c r="E159" t="b">
         <v>1</v>
       </c>
-      <c r="F159" s="3"/>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F159" s="3" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>37</v>
       </c>
@@ -5122,9 +5579,14 @@
       <c r="E160" t="b">
         <v>1</v>
       </c>
-      <c r="F160" s="3"/>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F160" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="G160" s="3" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>233</v>
       </c>
@@ -5140,9 +5602,11 @@
       <c r="E161" t="b">
         <v>1</v>
       </c>
-      <c r="F161" s="3"/>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F161" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>51</v>
       </c>
@@ -5158,9 +5622,11 @@
       <c r="E162" t="b">
         <v>1</v>
       </c>
-      <c r="F162" s="3"/>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F162" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>245</v>
       </c>
@@ -5176,9 +5642,14 @@
       <c r="E163" t="b">
         <v>1</v>
       </c>
-      <c r="F163" s="3"/>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F163" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="G163" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>303</v>
       </c>
@@ -5194,9 +5665,11 @@
       <c r="E164" t="b">
         <v>1</v>
       </c>
-      <c r="F164" s="3"/>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F164" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>215</v>
       </c>
@@ -5212,9 +5685,11 @@
       <c r="E165" t="b">
         <v>1</v>
       </c>
-      <c r="F165" s="3"/>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F165" s="3" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>59</v>
       </c>
@@ -5230,9 +5705,11 @@
       <c r="E166" t="b">
         <v>1</v>
       </c>
-      <c r="F166" s="3"/>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F166" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>25</v>
       </c>
@@ -5248,9 +5725,14 @@
       <c r="E167" t="b">
         <v>1</v>
       </c>
-      <c r="F167" s="3"/>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F167" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="G167" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>265</v>
       </c>
@@ -5266,9 +5748,11 @@
       <c r="E168" t="b">
         <v>1</v>
       </c>
-      <c r="F168" s="3"/>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F168" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>159</v>
       </c>
@@ -5284,9 +5768,11 @@
       <c r="E169" t="b">
         <v>1</v>
       </c>
-      <c r="F169" s="3"/>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F169" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>179</v>
       </c>
@@ -5302,9 +5788,11 @@
       <c r="E170" t="b">
         <v>1</v>
       </c>
-      <c r="F170" s="3"/>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F170" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>79</v>
       </c>
@@ -5320,7 +5808,9 @@
       <c r="E171" t="b">
         <v>1</v>
       </c>
-      <c r="F171" s="3"/>
+      <c r="F171" s="3" t="s">
+        <v>439</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E171">

</xml_diff>

<commit_message>
NSE-7719 - fill in Claire as admin on repos without one
</commit_message>
<xml_diff>
--- a/NEONScience/NEONScience_Repos.xlsx
+++ b/NEONScience/NEONScience_Repos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhayes\JIRA-Tickets\NSE-7719\NEONIT\NEONScience\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3F0C8E-CFAF-4607-9EBF-377572479EFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED4A52E-C5A6-4915-8CA0-B4FC8DE0F95F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="3210" windowWidth="28770" windowHeight="16170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4245" yWindow="2505" windowWidth="28770" windowHeight="16725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="newrepos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="445">
   <si>
     <t>Repo Name</t>
   </si>
@@ -1095,9 +1095,6 @@
   </si>
   <si>
     <t>David Durden</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>Claire Lunch
@@ -1297,9 +1294,6 @@
     <t>Guy Litt</t>
   </si>
   <si>
-    <t>NONE</t>
-  </si>
-  <si>
     <t>This was setup by Greg Holling and there is nothing in the repo</t>
   </si>
   <si>
@@ -1432,9 +1426,6 @@
 Eric Sokol</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>empty created by Lee Stanish</t>
   </si>
   <si>
@@ -1483,6 +1474,13 @@
   </si>
   <si>
     <t>Samantha Weintraub is the main committer</t>
+  </si>
+  <si>
+    <t>needs AOP member as admin?</t>
+  </si>
+  <si>
+    <t>Claire Lunch
+Elizabeth Hayes</t>
   </si>
 </sst>
 </file>
@@ -2333,8 +2331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F152" sqref="F152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2369,7 +2367,7 @@
         <v>345</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2653,7 +2651,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -2670,7 +2668,10 @@
         <v>1</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>356</v>
+        <v>366</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2690,7 +2691,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2710,7 +2711,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2730,7 +2731,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2750,7 +2751,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -2770,7 +2771,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2790,7 +2791,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -2810,7 +2811,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2830,7 +2831,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2850,7 +2851,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2870,7 +2871,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2890,7 +2891,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2910,7 +2911,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2930,7 +2931,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2970,7 +2971,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2990,7 +2991,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -3030,7 +3031,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3050,7 +3051,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3070,7 +3071,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -3110,7 +3111,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -3130,7 +3131,7 @@
         <v>1</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -3150,7 +3151,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -3170,7 +3171,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -3190,7 +3191,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3230,7 +3231,7 @@
         <v>1</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -3270,7 +3271,7 @@
         <v>1</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3290,7 +3291,7 @@
         <v>1</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -3310,7 +3311,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3330,7 +3331,7 @@
         <v>1</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3350,7 +3351,7 @@
         <v>1</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3370,7 +3371,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3390,7 +3391,7 @@
         <v>1</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3410,10 +3411,10 @@
         <v>1</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -3433,7 +3434,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3453,7 +3454,7 @@
         <v>1</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -3473,7 +3474,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3493,7 +3494,7 @@
         <v>1</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3533,7 +3534,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3573,7 +3574,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3593,7 +3594,7 @@
         <v>1</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3613,7 +3614,7 @@
         <v>1</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3633,7 +3634,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3653,7 +3654,7 @@
         <v>1</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3673,7 +3674,7 @@
         <v>1</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3693,7 +3694,7 @@
         <v>1</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3733,7 +3734,7 @@
         <v>1</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3753,7 +3754,7 @@
         <v>1</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3773,7 +3774,7 @@
         <v>1</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3793,7 +3794,7 @@
         <v>1</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3813,7 +3814,7 @@
         <v>1</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -3833,7 +3834,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -3893,7 +3894,7 @@
         <v>1</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -3913,7 +3914,7 @@
         <v>1</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -3933,7 +3934,7 @@
         <v>1</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3953,7 +3954,7 @@
         <v>1</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -3973,7 +3974,7 @@
         <v>1</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -4013,7 +4014,7 @@
         <v>1</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -4033,7 +4034,7 @@
         <v>1</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4053,7 +4054,7 @@
         <v>1</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4073,7 +4074,7 @@
         <v>1</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4093,10 +4094,10 @@
         <v>1</v>
       </c>
       <c r="F87" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="G87" s="3" t="s">
         <v>393</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4116,7 +4117,7 @@
         <v>1</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -4156,7 +4157,7 @@
         <v>1</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4176,7 +4177,7 @@
         <v>1</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4196,7 +4197,7 @@
         <v>1</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4216,7 +4217,7 @@
         <v>1</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4236,7 +4237,7 @@
         <v>1</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4256,7 +4257,7 @@
         <v>1</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -4276,7 +4277,7 @@
         <v>1</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4296,7 +4297,7 @@
         <v>1</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4316,7 +4317,7 @@
         <v>1</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -4336,7 +4337,7 @@
         <v>1</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4356,7 +4357,7 @@
         <v>1</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -4376,7 +4377,7 @@
         <v>1</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -4396,7 +4397,7 @@
         <v>1</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4416,10 +4417,10 @@
         <v>1</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4439,7 +4440,7 @@
         <v>1</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -4459,7 +4460,7 @@
         <v>1</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4479,7 +4480,7 @@
         <v>1</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -4499,7 +4500,7 @@
         <v>1</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4519,7 +4520,7 @@
         <v>1</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -4539,10 +4540,10 @@
         <v>1</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>404</v>
+        <v>444</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4562,7 +4563,7 @@
         <v>1</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4582,7 +4583,7 @@
         <v>1</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4602,7 +4603,7 @@
         <v>1</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4622,7 +4623,7 @@
         <v>1</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -4642,7 +4643,7 @@
         <v>1</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4662,10 +4663,10 @@
         <v>1</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -4685,7 +4686,7 @@
         <v>1</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -4705,10 +4706,10 @@
         <v>1</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -4728,7 +4729,7 @@
         <v>1</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -4748,7 +4749,7 @@
         <v>1</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -4768,10 +4769,10 @@
         <v>1</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -4791,7 +4792,7 @@
         <v>1</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4811,7 +4812,7 @@
         <v>1</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4831,7 +4832,7 @@
         <v>1</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4851,7 +4852,7 @@
         <v>1</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4871,7 +4872,7 @@
         <v>1</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -4891,7 +4892,7 @@
         <v>1</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4911,7 +4912,7 @@
         <v>1</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -4931,7 +4932,7 @@
         <v>1</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -4951,7 +4952,7 @@
         <v>1</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -4971,7 +4972,7 @@
         <v>1</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -4991,7 +4992,7 @@
         <v>1</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -5031,7 +5032,7 @@
         <v>1</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -5051,7 +5052,7 @@
         <v>1</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5071,7 +5072,7 @@
         <v>1</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5091,7 +5092,7 @@
         <v>1</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5111,7 +5112,7 @@
         <v>1</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -5131,7 +5132,7 @@
         <v>1</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -5151,7 +5152,7 @@
         <v>1</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5171,7 +5172,7 @@
         <v>1</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
@@ -5191,7 +5192,7 @@
         <v>1</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5211,7 +5212,7 @@
         <v>1</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5231,10 +5232,10 @@
         <v>1</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -5254,7 +5255,7 @@
         <v>1</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -5274,7 +5275,7 @@
         <v>1</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5294,7 +5295,7 @@
         <v>1</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -5314,7 +5315,7 @@
         <v>1</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -5354,7 +5355,7 @@
         <v>1</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5374,10 +5375,10 @@
         <v>1</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>433</v>
+        <v>366</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5397,7 +5398,7 @@
         <v>1</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5417,7 +5418,7 @@
         <v>1</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -5437,7 +5438,7 @@
         <v>1</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5457,10 +5458,10 @@
         <v>1</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="G154" s="3" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -5480,7 +5481,7 @@
         <v>1</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -5500,7 +5501,7 @@
         <v>1</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5520,7 +5521,7 @@
         <v>1</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
@@ -5540,7 +5541,7 @@
         <v>1</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5560,7 +5561,7 @@
         <v>1</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5580,10 +5581,10 @@
         <v>1</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="G160" s="3" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -5623,7 +5624,7 @@
         <v>1</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="163" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -5643,10 +5644,10 @@
         <v>1</v>
       </c>
       <c r="F163" s="3" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -5706,7 +5707,7 @@
         <v>1</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="167" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5726,10 +5727,10 @@
         <v>1</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G167" s="3" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -5769,7 +5770,7 @@
         <v>1</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="170" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5789,7 +5790,7 @@
         <v>1</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5809,7 +5810,7 @@
         <v>1</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>

</xml_diff>